<commit_message>
Cambios en la Docu
</commit_message>
<xml_diff>
--- a/material util/Presupuestos/Presupuesto De Costes.xlsx
+++ b/material util/Presupuestos/Presupuesto De Costes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Gómez\Desktop\tfg_inmobiliaria\material util\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Gómez\Desktop\tfg_inmobiliaria\material util\Presupuestos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57DEE9D-B99A-43CE-AF25-5FFE22B703D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3B2ED8-8901-4152-8B20-C69F14FD92C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
   <si>
     <t>Capítulo</t>
   </si>
@@ -426,7 +426,10 @@
     <t>Licencias</t>
   </si>
   <si>
-    <t>BENEFICIO (14%):</t>
+    <t>BENEFICIO (7%):</t>
+  </si>
+  <si>
+    <t>Fase de Pruebas</t>
   </si>
 </sst>
 </file>
@@ -759,21 +762,30 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -787,15 +799,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1085,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
-      <selection activeCell="S70" sqref="S70"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S68" sqref="S68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,19 +1114,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
@@ -1267,10 +1270,10 @@
         <v>161.93999999999997</v>
       </c>
       <c r="K6" s="27"/>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="N6" s="43"/>
+      <c r="N6" s="46"/>
     </row>
     <row r="7" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
@@ -1329,7 +1332,7 @@
         <v>50</v>
       </c>
       <c r="N8" s="1">
-        <v>7.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -1432,7 +1435,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4">
         <f>J14</f>
-        <v>1872.06</v>
+        <v>822.06000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -1451,7 +1454,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3">
         <f>SUM(G15:I19)</f>
-        <v>1872.06</v>
+        <v>822.06000000000006</v>
       </c>
       <c r="K14" s="3"/>
     </row>
@@ -1466,11 +1469,11 @@
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>450</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
@@ -1582,7 +1585,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4">
         <f>SUM(J21:J50)</f>
-        <v>2505</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1601,7 +1604,7 @@
       <c r="I21" s="27"/>
       <c r="J21" s="3">
         <f>SUM(I22:I25)</f>
-        <v>210</v>
+        <v>90</v>
       </c>
       <c r="K21" s="27"/>
     </row>
@@ -1618,11 +1621,11 @@
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I22" s="29">
         <f>H22*$N$8</f>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="29"/>
@@ -1644,7 +1647,7 @@
       </c>
       <c r="I23" s="29">
         <f t="shared" ref="I23:I50" si="1">H23*$N$8</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="29"/>
@@ -1662,11 +1665,11 @@
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I24" s="29">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="29"/>
@@ -1684,11 +1687,11 @@
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I25" s="29">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="29"/>
@@ -1709,7 +1712,7 @@
       <c r="I26" s="27"/>
       <c r="J26" s="3">
         <f>SUM(I27:I31)</f>
-        <v>435</v>
+        <v>195</v>
       </c>
       <c r="K26" s="27"/>
     </row>
@@ -1730,7 +1733,7 @@
       </c>
       <c r="I27" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="29"/>
@@ -1748,11 +1751,11 @@
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
       <c r="H28" s="29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I28" s="29">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="29"/>
@@ -1770,11 +1773,11 @@
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I29" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="29"/>
@@ -1792,11 +1795,11 @@
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
       <c r="H30" s="29">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I30" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="29"/>
@@ -1814,11 +1817,11 @@
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
       <c r="H31" s="29">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I31" s="29">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="29"/>
@@ -1839,7 +1842,7 @@
       <c r="I32" s="27"/>
       <c r="J32" s="3">
         <f>SUM(I33:I35)</f>
-        <v>360</v>
+        <v>90</v>
       </c>
       <c r="K32" s="27"/>
     </row>
@@ -1856,11 +1859,11 @@
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="29">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I33" s="29">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="29"/>
@@ -1878,11 +1881,11 @@
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
       <c r="H34" s="29">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="I34" s="29">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="29"/>
@@ -1900,11 +1903,11 @@
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
       <c r="H35" s="29">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I35" s="29">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="29"/>
@@ -1925,7 +1928,7 @@
       <c r="I36" s="27"/>
       <c r="J36" s="3">
         <f>SUM(I37:I42)</f>
-        <v>765</v>
+        <v>400</v>
       </c>
       <c r="K36" s="27"/>
     </row>
@@ -1946,7 +1949,7 @@
       </c>
       <c r="I37" s="29">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="29"/>
@@ -1964,11 +1967,11 @@
       <c r="F38" s="29"/>
       <c r="G38" s="29"/>
       <c r="H38" s="29">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I38" s="29">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="29"/>
@@ -1986,11 +1989,11 @@
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="29">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I39" s="29">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="29"/>
@@ -2008,11 +2011,11 @@
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
       <c r="H40" s="29">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I40" s="29">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="29"/>
@@ -2030,11 +2033,11 @@
       <c r="F41" s="29"/>
       <c r="G41" s="29"/>
       <c r="H41" s="29">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I41" s="29">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="29"/>
@@ -2056,7 +2059,7 @@
       </c>
       <c r="I42" s="29">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="29"/>
@@ -2068,7 +2071,7 @@
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="24" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
@@ -2077,7 +2080,7 @@
       <c r="I43" s="27"/>
       <c r="J43" s="3">
         <f>SUM(I44:I46)</f>
-        <v>405</v>
+        <v>190</v>
       </c>
       <c r="K43" s="27"/>
     </row>
@@ -2094,11 +2097,11 @@
       <c r="F44" s="29"/>
       <c r="G44" s="29"/>
       <c r="H44" s="29">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I44" s="29">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="29"/>
@@ -2116,11 +2119,11 @@
       <c r="F45" s="29"/>
       <c r="G45" s="29"/>
       <c r="H45" s="29">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I45" s="29">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="29"/>
@@ -2142,7 +2145,7 @@
       </c>
       <c r="I46" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="29"/>
@@ -2163,7 +2166,7 @@
       <c r="I47" s="27"/>
       <c r="J47" s="3">
         <f>SUM(I48:I50)</f>
-        <v>330</v>
+        <v>145</v>
       </c>
       <c r="K47" s="27"/>
     </row>
@@ -2180,11 +2183,11 @@
       <c r="F48" s="29"/>
       <c r="G48" s="29"/>
       <c r="H48" s="29">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I48" s="29">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="29"/>
@@ -2202,11 +2205,11 @@
       <c r="F49" s="29"/>
       <c r="G49" s="29"/>
       <c r="H49" s="29">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I49" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="29"/>
@@ -2224,75 +2227,75 @@
       <c r="F50" s="29"/>
       <c r="G50" s="29"/>
       <c r="H50" s="29">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I50" s="29">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="J50" s="29"/>
       <c r="K50" s="29"/>
     </row>
     <row r="51" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="45">
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="37">
         <f>SUM(K3:K20)</f>
-        <v>4741.25</v>
-      </c>
-      <c r="K51" s="46"/>
+        <v>2296.25</v>
+      </c>
+      <c r="K51" s="38"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
+      <c r="A52" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="45">
-        <f>J51*0.14</f>
-        <v>663.77500000000009</v>
-      </c>
-      <c r="K52" s="46"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="37">
+        <f>J51*0.07</f>
+        <v>160.73750000000001</v>
+      </c>
+      <c r="K52" s="38"/>
     </row>
     <row r="53" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
       <c r="I53" s="32"/>
-      <c r="J53" s="45">
+      <c r="J53" s="37">
         <f>J51+J52</f>
-        <v>5405.0249999999996</v>
-      </c>
-      <c r="K53" s="46"/>
+        <v>2456.9875000000002</v>
+      </c>
+      <c r="K53" s="38"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="R56" s="44" t="s">
+      <c r="R56" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="S56" s="44"/>
-      <c r="T56" s="44"/>
+      <c r="S56" s="34"/>
+      <c r="T56" s="34"/>
     </row>
     <row r="57" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="R57" s="4" t="s">
@@ -2326,7 +2329,7 @@
       </c>
       <c r="T58" s="3">
         <f>T59+T60</f>
-        <v>2236.25</v>
+        <v>1186.25</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -2346,7 +2349,7 @@
       <c r="S60" s="29"/>
       <c r="T60" s="29">
         <f>J10+J14</f>
-        <v>2042.06</v>
+        <v>992.06000000000006</v>
       </c>
     </row>
     <row r="61" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -2354,7 +2357,7 @@
         <v>118</v>
       </c>
       <c r="S61" s="3">
-        <v>755.6</v>
+        <v>285</v>
       </c>
       <c r="T61" s="3">
         <v>0</v>
@@ -2365,7 +2368,7 @@
         <v>119</v>
       </c>
       <c r="S62" s="3">
-        <v>515.5</v>
+        <v>90</v>
       </c>
       <c r="T62" s="3">
         <v>0</v>
@@ -2377,7 +2380,7 @@
       </c>
       <c r="S63" s="3">
         <f>SUM(S64:S68)</f>
-        <v>1500.92</v>
+        <v>560.74</v>
       </c>
       <c r="T63" s="3">
         <f>SUM(T64:T68)</f>
@@ -2389,7 +2392,7 @@
         <v>121</v>
       </c>
       <c r="S64" s="29">
-        <v>326.64</v>
+        <v>132.5</v>
       </c>
       <c r="T64" s="29"/>
     </row>
@@ -2398,7 +2401,7 @@
         <v>77</v>
       </c>
       <c r="S65" s="29">
-        <v>378.23</v>
+        <v>132</v>
       </c>
       <c r="T65" s="29"/>
     </row>
@@ -2407,7 +2410,7 @@
         <v>122</v>
       </c>
       <c r="S66" s="29">
-        <v>316.08999999999997</v>
+        <v>132.19999999999999</v>
       </c>
       <c r="T66" s="29"/>
     </row>
@@ -2416,7 +2419,7 @@
         <v>123</v>
       </c>
       <c r="S67" s="29">
-        <v>234.51</v>
+        <v>92.04</v>
       </c>
       <c r="T67" s="29"/>
     </row>
@@ -2425,7 +2428,7 @@
         <v>124</v>
       </c>
       <c r="S68" s="29">
-        <v>245.45</v>
+        <v>72</v>
       </c>
       <c r="T68" s="29"/>
     </row>
@@ -2434,7 +2437,7 @@
         <v>125</v>
       </c>
       <c r="S69" s="3">
-        <v>325.39999999999998</v>
+        <v>190</v>
       </c>
       <c r="T69" s="3">
         <v>0</v>
@@ -2445,7 +2448,7 @@
         <v>126</v>
       </c>
       <c r="S70" s="3">
-        <v>71.36</v>
+        <v>145</v>
       </c>
       <c r="T70" s="3">
         <v>0</v>
@@ -2457,35 +2460,35 @@
       </c>
       <c r="S71" s="23">
         <f>S58+S61+S62+S63+S69+S70</f>
-        <v>3168.78</v>
+        <v>1270.74</v>
       </c>
       <c r="T71" s="23">
         <f>T58+T61+T62+T63+T69+T70</f>
-        <v>2236.25</v>
+        <v>1186.25</v>
       </c>
     </row>
     <row r="72" spans="18:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="R72" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="S72" s="36">
+      <c r="S72" s="35">
         <f>S71+T71</f>
-        <v>5405.0300000000007</v>
-      </c>
-      <c r="T72" s="38"/>
+        <v>2456.9899999999998</v>
+      </c>
+      <c r="T72" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="R56:T56"/>
     <mergeCell ref="S72:T72"/>
     <mergeCell ref="J51:K51"/>
     <mergeCell ref="J52:K52"/>
     <mergeCell ref="J53:K53"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>